<commit_message>
updated maps and spatial regression. added an alias look up table. Facet grid order does not obey
</commit_message>
<xml_diff>
--- a/input_data/var_alias_lookup.xlsx
+++ b/input_data/var_alias_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlocke/BaltimoreGIS/iTree/Trini/BaltimoreStreetTreeProject/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FC4ACE5-C0AD-A048-BA2A-854CC141B5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0070B4-962B-B240-8C97-4CED9A7A7AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="3120" windowWidth="27640" windowHeight="16940" xr2:uid="{FFD208E8-B45E-E34B-AB84-CE27C1CE0980}"/>
+    <workbookView xWindow="9700" yWindow="5580" windowWidth="20680" windowHeight="14500" xr2:uid="{FFD208E8-B45E-E34B-AB84-CE27C1CE0980}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>var</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Vacant and abandoned residential properties</t>
   </si>
   <si>
-    <t>Total NB area</t>
-  </si>
-  <si>
     <t>Total road length (not including highways)</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
     <t>Population density</t>
   </si>
   <si>
-    <t>ave_temp</t>
-  </si>
-  <si>
     <t>mhhi20</t>
   </si>
   <si>
@@ -127,9 +121,6 @@
     <t>PopDensity</t>
   </si>
   <si>
-    <t>include</t>
-  </si>
-  <si>
     <t>PercentImp</t>
   </si>
   <si>
@@ -154,14 +145,89 @@
     <t>Perc2.97</t>
   </si>
   <si>
-    <t>percenet_filled</t>
+    <t>Evar</t>
+  </si>
+  <si>
+    <t>AvgDBH_smallmed</t>
+  </si>
+  <si>
+    <t>AvgDBH_large</t>
+  </si>
+  <si>
+    <t>spave</t>
+  </si>
+  <si>
+    <t>percent_filled</t>
+  </si>
+  <si>
+    <t>rich_tottree</t>
+  </si>
+  <si>
+    <t>alias2</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>avg_temp</t>
+  </si>
+  <si>
+    <t>Percent White</t>
+  </si>
+  <si>
+    <t>Percent Black</t>
+  </si>
+  <si>
+    <t>Educational Attainment</t>
+  </si>
+  <si>
+    <t>Vacancy</t>
+  </si>
+  <si>
+    <t>Percent Impervious</t>
+  </si>
+  <si>
+    <t>Pop Density</t>
+  </si>
+  <si>
+    <t>Road length</t>
+  </si>
+  <si>
+    <t>Rel. Richness</t>
+  </si>
+  <si>
+    <t>Beta Diversity</t>
+  </si>
+  <si>
+    <t>DBH small</t>
+  </si>
+  <si>
+    <t>DBH large</t>
+  </si>
+  <si>
+    <t>% target pit</t>
+  </si>
+  <si>
+    <t>Good Condition</t>
+  </si>
+  <si>
+    <t>Poor Condition</t>
+  </si>
+  <si>
+    <t>Dead</t>
+  </si>
+  <si>
+    <t>Stocking</t>
+  </si>
+  <si>
+    <t>totsites</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -174,6 +240,13 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -196,9 +269,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,14 +590,15 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="61" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="4" max="4" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -537,17 +612,20 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>39</v>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -555,7 +633,13 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
       <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -563,15 +647,27 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
       <c r="C5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -579,7 +675,13 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
       <c r="C6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -587,7 +689,13 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
       <c r="C7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -596,9 +704,12 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -607,9 +718,12 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -618,9 +732,12 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -629,120 +746,144 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
       <c r="C16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>50</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D20" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
       <c r="B21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
massive consistent labelings update.
</commit_message>
<xml_diff>
--- a/input_data/var_alias_lookup.xlsx
+++ b/input_data/var_alias_lookup.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlocke/BaltimoreGIS/iTree/Trini/BaltimoreStreetTreeProject/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0070B4-962B-B240-8C97-4CED9A7A7AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F1B2E3-2A75-824D-8F52-B848C1EAC849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9700" yWindow="5580" windowWidth="20680" windowHeight="14500" xr2:uid="{FFD208E8-B45E-E34B-AB84-CE27C1CE0980}"/>
+    <workbookView xWindow="6660" yWindow="1880" windowWidth="23180" windowHeight="16640" xr2:uid="{FFD208E8-B45E-E34B-AB84-CE27C1CE0980}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>var</t>
   </si>
@@ -166,68 +166,82 @@
     <t>alias2</t>
   </si>
   <si>
-    <t>Income</t>
-  </si>
-  <si>
     <t>avg_temp</t>
   </si>
   <si>
-    <t>Percent White</t>
-  </si>
-  <si>
-    <t>Percent Black</t>
-  </si>
-  <si>
-    <t>Educational Attainment</t>
-  </si>
-  <si>
-    <t>Vacancy</t>
-  </si>
-  <si>
-    <t>Percent Impervious</t>
-  </si>
-  <si>
-    <t>Pop Density</t>
-  </si>
-  <si>
-    <t>Road length</t>
-  </si>
-  <si>
-    <t>Rel. Richness</t>
-  </si>
-  <si>
-    <t>Beta Diversity</t>
-  </si>
-  <si>
-    <t>DBH small</t>
-  </si>
-  <si>
-    <t>DBH large</t>
-  </si>
-  <si>
-    <t>% target pit</t>
-  </si>
-  <si>
-    <t>Good Condition</t>
-  </si>
-  <si>
-    <t>Poor Condition</t>
-  </si>
-  <si>
-    <t>Dead</t>
-  </si>
-  <si>
-    <t>Stocking</t>
-  </si>
-  <si>
     <t>totsites</t>
+  </si>
+  <si>
+    <t>Potential sites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black population (%) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">White population (%) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air Temperature (°C) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vacancy (%) </t>
+  </si>
+  <si>
+    <t>Impervious surface cover (%)</t>
+  </si>
+  <si>
+    <t>Road length (m)</t>
+  </si>
+  <si>
+    <t>Stocking (%)</t>
+  </si>
+  <si>
+    <t>Sites Above Target Pit Size (%)</t>
+  </si>
+  <si>
+    <t>Relative Species Richness</t>
+  </si>
+  <si>
+    <t>Poor Condition (%)</t>
+  </si>
+  <si>
+    <t>Good Condition (%)</t>
+  </si>
+  <si>
+    <t>Dead (%)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">β </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Diversity</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Bachelor’s Degree Educational Attainment (%) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Median household Income (USD) </t>
+  </si>
+  <si>
+    <t>Average DBH of Small Species (cm)</t>
+  </si>
+  <si>
+    <t>Average DBH of Large Species (cm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -247,6 +261,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -269,10 +289,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,15 +610,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD96809-3836-544D-B9D5-2FBA49BE8038}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="3" max="3" width="37" customWidth="1"/>
     <col min="4" max="4" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -623,7 +644,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -637,7 +658,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
@@ -664,8 +685,8 @@
       <c r="B5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>53</v>
+      <c r="C5" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -679,7 +700,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
@@ -693,7 +714,7 @@
         <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
@@ -707,7 +728,7 @@
         <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
@@ -721,7 +742,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
@@ -735,7 +756,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -749,7 +770,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>12</v>
@@ -763,7 +784,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>14</v>
@@ -791,7 +812,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
@@ -805,7 +826,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
@@ -819,7 +840,7 @@
         <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>18</v>
@@ -833,7 +854,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>24</v>
@@ -861,7 +882,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>20</v>
@@ -872,18 +893,24 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>44</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed pct_9m2 to pct_2.97
</commit_message>
<xml_diff>
--- a/input_data/var_alias_lookup.xlsx
+++ b/input_data/var_alias_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlocke/BaltimoreGIS/iTree/Trini/BaltimoreStreetTreeProject/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5131AB-2FE8-E440-B3A5-A66949310BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C313BAA1-F3D7-9747-A681-9933A85B9990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45620" yWindow="6440" windowWidth="23180" windowHeight="16640" xr2:uid="{FFD208E8-B45E-E34B-AB84-CE27C1CE0980}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{FFD208E8-B45E-E34B-AB84-CE27C1CE0980}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>PercGood</t>
   </si>
   <si>
-    <t>Perc2.97</t>
-  </si>
-  <si>
     <t>Evar</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>Rarefied richness</t>
+  </si>
+  <si>
+    <t>pct_9m2</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,7 +633,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -641,10 +641,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -655,13 +655,13 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -669,7 +669,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -683,10 +683,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -697,10 +697,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
@@ -711,10 +711,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
@@ -725,10 +725,10 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
@@ -742,7 +742,7 @@
         <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
@@ -756,7 +756,7 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
@@ -770,7 +770,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -784,7 +784,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -798,7 +798,7 @@
         <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>14</v>
@@ -812,7 +812,7 @@
         <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>15</v>
@@ -826,7 +826,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>16</v>
@@ -840,7 +840,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
@@ -868,7 +868,7 @@
         <v>28</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>18</v>
@@ -882,7 +882,7 @@
         <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>19</v>
@@ -893,10 +893,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>20</v>
@@ -907,10 +907,10 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>